<commit_message>
Change instruction set, language ideas, added font file.
</commit_message>
<xml_diff>
--- a/Instruction Set.xlsx
+++ b/Instruction Set.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse\OneDrive - BYU Office 365\Projects\AmberOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5E5AB293-3E9B-4E03-9659-5ED49B3ECFE3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version 0.00" sheetId="1" r:id="rId1"/>
     <sheet name="Version 0.01" sheetId="3" r:id="rId2"/>
     <sheet name="Testing" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="147">
   <si>
     <t>OpCode</t>
   </si>
@@ -433,13 +434,46 @@
     <t>error</t>
   </si>
   <si>
-    <t>16 byte computer</t>
+    <t>NOOP</t>
+  </si>
+  <si>
+    <t>16 bit computer</t>
+  </si>
+  <si>
+    <t>v-ram</t>
+  </si>
+  <si>
+    <t>NBLK</t>
+  </si>
+  <si>
+    <t>Goes to address 0 of next block</t>
+  </si>
+  <si>
+    <t>BLK</t>
+  </si>
+  <si>
+    <t>[OpCode, Block]</t>
+  </si>
+  <si>
+    <t>Goes to address 0 of specified block</t>
+  </si>
+  <si>
+    <t>BLKP</t>
+  </si>
+  <si>
+    <t>Goes to specified address of a specific block</t>
+  </si>
+  <si>
+    <t>[OpCode, Block, Address]</t>
+  </si>
+  <si>
+    <t>CHBLK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00\ 00\ 00\ 00"/>
   </numFmts>
@@ -597,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -654,6 +688,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -935,7 +975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I257"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
@@ -4032,11 +4072,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L257"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4055,7 +4095,7 @@
     <col min="12" max="16384" width="9.1796875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -4078,7 +4118,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="11">
         <v>0</v>
       </c>
@@ -4086,8 +4126,8 @@
         <f>DEC2BIN(ROW()-2,8)</f>
         <v>00000000</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>10</v>
+      <c r="C2" s="20" t="s">
+        <v>135</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>11</v>
@@ -4103,7 +4143,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -4128,7 +4168,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -4152,8 +4192,11 @@
       <c r="G4" s="11" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N4" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -4178,10 +4221,17 @@
         <v>109</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+      <c r="L5" s="8">
+        <f>POWER(2,16)</f>
+        <v>65536</v>
+      </c>
+      <c r="N5" s="21">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -4205,8 +4255,11 @@
       <c r="G6" s="11" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L6" s="8">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -4224,14 +4277,14 @@
         <v>57</v>
       </c>
       <c r="F7" s="11">
-        <f t="shared" ref="F7:F45" si="2">(LEN(E7)-LEN(SUBSTITUTE(E7, ",","")))/LEN(",")+1</f>
+        <f t="shared" ref="F7:F48" si="2">(LEN(E7)-LEN(SUBSTITUTE(E7, ",","")))/LEN(",")+1</f>
         <v>4</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -4256,7 +4309,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -4282,7 +4335,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>8</v>
       </c>
@@ -4317,7 +4370,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>9</v>
       </c>
@@ -4344,7 +4397,7 @@
       </c>
       <c r="I11" s="9">
         <f>AVERAGE(F:F)</f>
-        <v>3.5</v>
+        <v>3.4042553191489362</v>
       </c>
       <c r="K11" s="18" t="s">
         <v>132</v>
@@ -4353,7 +4406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>10</v>
       </c>
@@ -4385,7 +4438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>11</v>
       </c>
@@ -4414,7 +4467,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>12</v>
       </c>
@@ -4444,7 +4497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
         <v>13</v>
       </c>
@@ -4470,7 +4523,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="11">
         <v>14</v>
       </c>
@@ -5254,6 +5307,22 @@
         <f t="shared" si="0"/>
         <v>00101100</v>
       </c>
+      <c r="C46" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="11">
@@ -5263,6 +5332,22 @@
         <f t="shared" si="0"/>
         <v>00101101</v>
       </c>
+      <c r="C47" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="F47" s="11">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G47" s="20" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="11">
@@ -5272,8 +5357,24 @@
         <f t="shared" si="0"/>
         <v>00101110</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F48" s="11">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G48" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="11">
         <v>47</v>
       </c>
@@ -5281,8 +5382,11 @@
         <f t="shared" si="0"/>
         <v>00101111</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49" s="20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="11">
         <v>48</v>
       </c>
@@ -5291,7 +5395,7 @@
         <v>00110000</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="11">
         <v>49</v>
       </c>
@@ -5300,7 +5404,7 @@
         <v>00110001</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="11">
         <v>50</v>
       </c>
@@ -5309,7 +5413,7 @@
         <v>00110010</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="11">
         <v>51</v>
       </c>
@@ -5318,7 +5422,7 @@
         <v>00110011</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="11">
         <v>52</v>
       </c>
@@ -5327,7 +5431,7 @@
         <v>00110100</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="11">
         <v>53</v>
       </c>
@@ -5336,7 +5440,7 @@
         <v>00110101</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="11">
         <v>54</v>
       </c>
@@ -5345,7 +5449,7 @@
         <v>00110110</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="11">
         <v>55</v>
       </c>
@@ -5354,7 +5458,7 @@
         <v>00110111</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="11">
         <v>56</v>
       </c>
@@ -5363,7 +5467,7 @@
         <v>00111000</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="11">
         <v>57</v>
       </c>
@@ -5372,7 +5476,7 @@
         <v>00111001</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="11">
         <v>58</v>
       </c>
@@ -5381,7 +5485,7 @@
         <v>00111010</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="11">
         <v>59</v>
       </c>
@@ -5390,7 +5494,7 @@
         <v>00111011</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="11">
         <v>60</v>
       </c>
@@ -5399,7 +5503,7 @@
         <v>00111100</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="11">
         <v>61</v>
       </c>
@@ -5408,7 +5512,7 @@
         <v>00111101</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="11">
         <v>62</v>
       </c>
@@ -7161,7 +7265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>